<commit_message>
Atualização automática de TRES_PASSOS.xlsx
</commit_message>
<xml_diff>
--- a/TRES_PASSOS.xlsx
+++ b/TRES_PASSOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C421D046-2D1F-4082-BA3F-7A0FEE93E30C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01211825-49B9-4E83-8972-070D452FA5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,7 +1219,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{1D7DA0A3-327F-4156-A2D2-A00A5191E2D6}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{91D24FA0-19CA-4A84-8377-B536444C9102}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1249,10 +1249,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A828F723-8888-4AA0-AA0B-63A2269DA22D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8747832E-A896-4499-B757-119000288020}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1290,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4849EACD-3C97-47CF-821A-30CEF72BB9AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8931266-6696-4B96-BEBB-714A7CAD37BE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1353,7 +1353,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90261DD7-CD36-4B25-8201-5D5CD2B0D962}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F657D67-54EF-4E61-B6D1-05A601A20FE4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1372,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79E983D9-21A7-96C4-4E86-4E868F1773CD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4001DBA-D6D1-9EF7-16AD-0DB129DFB7C2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1421,7 +1421,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFC0D71D-56DD-62C7-FD39-36EACD603CAA}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9089F8AB-EBDE-7D30-A56D-C5548FD6CE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1440,7 +1440,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318C77F0-AFCB-A0EF-1E47-469DD7A45C43}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D3EEC2F-40F7-C8B5-8C4D-D10C17CF81C3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1471,7 +1471,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7E80804-440A-8817-5AC6-E50B9D691772}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D8134BE-B976-AD46-07AD-FB7BDE4FF0D5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1502,7 +1502,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB426B66-4478-4D97-02DC-981B51638573}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20514325-F683-CAC7-3D01-31D3F9176F99}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1545,7 +1545,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{039E63EE-1B6B-4485-A52D-C3B052475F2D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F9CE961-3164-4AF6-8DD6-5DD5390182A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1583,7 +1583,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C7AE2E-CEAF-4602-B7AD-47C993086966}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E424E09C-D475-4DFB-8328-36C33143DE8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1626,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E6DD0C3-E97B-40EF-9246-345214894F5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{992657EA-51FF-4F75-95AC-E1D76FB9F54F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1939,7 +1939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71898023-A57C-44E1-98FC-7710175A2456}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A3542B-096E-480B-959A-DCB83655431B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>